<commit_message>
changes done in existing programs
</commit_message>
<xml_diff>
--- a/testdata/userdata.xlsx
+++ b/testdata/userdata.xlsx
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O10"/>
+  <oleSize ref="A1:E10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>CustomerName</t>
   </si>
@@ -49,19 +49,26 @@
     <t>pass</t>
   </si>
   <si>
-    <t>fbgfhngfj</t>
-  </si>
-  <si>
     <t>vdggdsgfdhfdgdgfdgt</t>
   </si>
   <si>
     <t>BillName</t>
+  </si>
+  <si>
+    <t>1 billing type has been successfully added.</t>
+  </si>
+  <si>
+    <t>mhgfxxfbchgj</t>
+  </si>
+  <si>
+    <t>Creditcatrd14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,12 +119,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +438,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="48.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -452,7 +460,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -483,15 +491,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="39.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -513,10 +521,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -546,30 +554,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="46.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>